<commit_message>
updated maturity agreement tables to have total sums
</commit_message>
<xml_diff>
--- a/tables/Table_S1.xlsx
+++ b/tables/Table_S1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markusmin/Documents/Hollings_NOAA/macro_histo_maturity/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8EE3245F-5128-2E49-AC1D-BD3F85AF6C95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{537A1624-0457-5E4A-A738-8058C59F35B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2120" yWindow="460" windowWidth="27240" windowHeight="16440" xr2:uid="{9D08F7DC-992A-CE41-A646-883C57DC637D}"/>
+    <workbookView xWindow="7860" yWindow="460" windowWidth="27240" windowHeight="16440" xr2:uid="{9D08F7DC-992A-CE41-A646-883C57DC637D}"/>
   </bookViews>
   <sheets>
     <sheet name="canary_rockfish" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="66">
   <si>
     <t>time_period</t>
   </si>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>0.5 (0.05)</t>
+  </si>
+  <si>
+    <t>plusminusCI95</t>
   </si>
 </sst>
 </file>
@@ -580,24 +583,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BD5FC18-6034-034E-8BBE-D2CAD903A58B}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -614,16 +608,19 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -639,17 +636,20 @@
       <c r="E2">
         <v>45.96</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2">
+        <v>0.37</v>
+      </c>
+      <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -665,17 +665,20 @@
       <c r="E3">
         <v>46.37</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3">
+        <v>0.4</v>
+      </c>
+      <c r="G3" t="s">
         <v>14</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>15</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -691,17 +694,20 @@
       <c r="E4">
         <v>46.74</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="G4" t="s">
         <v>17</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>18</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -717,17 +723,20 @@
       <c r="E5">
         <v>47.95</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5">
+        <v>1.37</v>
+      </c>
+      <c r="G5" t="s">
         <v>20</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>21</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -743,17 +752,20 @@
       <c r="E6">
         <v>32.659999999999997</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6">
+        <v>0.2</v>
+      </c>
+      <c r="G6" t="s">
         <v>24</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>25</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -769,17 +781,20 @@
       <c r="E7">
         <v>40.090000000000003</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7">
+        <v>0.42</v>
+      </c>
+      <c r="G7" t="s">
         <v>27</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>28</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -795,17 +810,20 @@
       <c r="E8">
         <v>33.380000000000003</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8">
+        <v>1.29</v>
+      </c>
+      <c r="G8" t="s">
         <v>30</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>31</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -821,13 +839,16 @@
       <c r="E9">
         <v>42.31</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9">
+        <v>4.05</v>
+      </c>
+      <c r="G9" t="s">
         <v>33</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>34</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>35</v>
       </c>
     </row>
@@ -838,25 +859,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F92B080-2F10-E842-B6D8-92C970F1A283}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -876,16 +887,19 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -904,17 +918,20 @@
       <c r="F2">
         <v>55.17</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2">
+        <v>0.61</v>
+      </c>
+      <c r="H2" t="s">
         <v>38</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>39</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -933,17 +950,20 @@
       <c r="F3">
         <v>55.44</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3">
+        <v>0.59</v>
+      </c>
+      <c r="H3" t="s">
         <v>41</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>42</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -962,17 +982,20 @@
       <c r="F4">
         <v>58.52</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4">
+        <v>0.88</v>
+      </c>
+      <c r="H4" t="s">
         <v>44</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>45</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -991,17 +1014,20 @@
       <c r="F5">
         <v>55.55</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5">
+        <v>1.45</v>
+      </c>
+      <c r="H5" t="s">
         <v>47</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>48</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -1020,17 +1046,20 @@
       <c r="F6">
         <v>56.01</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6">
+        <v>1.64</v>
+      </c>
+      <c r="H6" t="s">
         <v>50</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>51</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -1049,17 +1078,20 @@
       <c r="F7">
         <v>48.44</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H7" t="s">
         <v>54</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>55</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -1078,17 +1110,20 @@
       <c r="F8">
         <v>48.44</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H8" t="s">
         <v>54</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>55</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -1107,17 +1142,20 @@
       <c r="F9">
         <v>54.82</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9">
+        <v>0.5</v>
+      </c>
+      <c r="H9" t="s">
         <v>56</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>57</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -1136,17 +1174,20 @@
       <c r="F10">
         <v>49.25</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10">
+        <v>0.49</v>
+      </c>
+      <c r="H10" t="s">
         <v>59</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>60</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -1165,13 +1206,16 @@
       <c r="F11">
         <v>55.12</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11">
+        <v>0.88</v>
+      </c>
+      <c r="H11" t="s">
         <v>62</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>63</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>